<commit_message>
updated models and views
</commit_message>
<xml_diff>
--- a/resources/ModelPlans.xlsx
+++ b/resources/ModelPlans.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
-    <sheet name="views" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="views" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -82,6 +83,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Larry:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I have a question on user model profiles or types. </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -111,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>make</t>
   </si>
@@ -299,14 +324,17 @@
     <t>Length of time since last serviced Years_? Month_?</t>
   </si>
   <si>
-    <t>Service class: Neccessity?</t>
+    <t>Service class: Neccessary?</t>
+  </si>
+  <si>
+    <t>&lt;---foreign key---user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +377,19 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -713,7 +754,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,7 +1028,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="7:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17"/>
       <c r="G17" s="6" t="s">
         <v>61</v>
       </c>
@@ -1000,10 +1042,222 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17"/>
+      <c r="G17" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added more fields to account/model
</commit_message>
<xml_diff>
--- a/resources/ModelPlans.xlsx
+++ b/resources/ModelPlans.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="model2" sheetId="3" r:id="rId2"/>
     <sheet name="views" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>make</t>
   </si>
@@ -352,186 +352,6 @@
   </si>
   <si>
     <t xml:space="preserve">        )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ),</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Video'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0C4B33"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, (</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">            (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'vhs'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0C4B33"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'VHS Tape'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0C4B33"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>),</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">            (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'dvd'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0C4B33"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'DVD'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0C4B33"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>),</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'unknown'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0C4B33"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBA2121"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Unknown'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0C4B33"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="1"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>),</t>
-    </r>
-  </si>
-  <si>
-    <t>)</t>
   </si>
   <si>
     <r>
@@ -1236,9 +1056,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1529,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1720,7 +1540,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
         <v>29</v>
@@ -1728,7 +1548,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E12" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
         <v>30</v>
@@ -1736,7 +1556,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E13" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
         <v>63</v>
@@ -1744,17 +1564,17 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E14" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E15" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E16" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -1764,45 +1584,31 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E18" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19"/>
-      <c r="E19" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="E19" s="7"/>
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E24" s="7" t="s">
-        <v>76</v>
-      </c>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E25" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="E25" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1814,7 +1620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Service_Request class to models
</commit_message>
<xml_diff>
--- a/resources/ModelPlans.xlsx
+++ b/resources/ModelPlans.xlsx
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
   <si>
     <t>make</t>
   </si>
@@ -629,13 +629,25 @@
   </si>
   <si>
     <t>Get all necessary fields related to User</t>
+  </si>
+  <si>
+    <t>Plan use of QuerySets ; https://docs.djangoproject.com/en/1.11/ref/models/querysets/</t>
+  </si>
+  <si>
+    <t>Service Record class</t>
+  </si>
+  <si>
+    <t>QuerySets</t>
+  </si>
+  <si>
+    <t>Piano Key Services</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,8 +728,16 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,6 +768,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -761,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -784,6 +810,8 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1393,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,8 +1432,8 @@
     <col min="4" max="4" width="40.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.44140625" customWidth="1"/>
     <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+    <col min="8" max="8" width="74" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1429,7 +1457,7 @@
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1448,8 +1476,8 @@
       <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
-        <v>58</v>
+      <c r="H2" s="12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1468,8 +1496,8 @@
       <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
-        <v>59</v>
+      <c r="H3" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1485,11 +1513,11 @@
       <c r="E4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1505,11 +1533,8 @@
       <c r="E5" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
+      <c r="H5" s="13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1524,10 +1549,10 @@
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
+        <v>10</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1543,11 +1568,11 @@
       <c r="E7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>60</v>
+      <c r="F7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1559,10 +1584,10 @@
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1573,7 +1598,10 @@
         <v>70</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1585,7 +1613,7 @@
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1599,7 +1627,10 @@
         <v>72</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>29</v>
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1610,7 +1641,7 @@
         <v>73</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1621,7 +1652,7 @@
         <v>74</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1631,6 +1662,9 @@
       <c r="E14" s="9" t="s">
         <v>75</v>
       </c>
+      <c r="F14" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D15" s="6" t="s">
@@ -1638,6 +1672,9 @@
       </c>
       <c r="E15" s="9" t="s">
         <v>76</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>